<commit_message>
Some old code, some new code.
</commit_message>
<xml_diff>
--- a/GM_2015-11-10.xlsx
+++ b/GM_2015-11-10.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AV$391</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AV$378</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1816,11 +1816,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV390"/>
+  <dimension ref="A1:AV377"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN22" sqref="AN22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A276" sqref="A276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19778,18 +19778,15 @@
     <row r="274" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN274" s="1"/>
     </row>
+    <row r="275" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN275" s="1"/>
+    </row>
     <row r="276" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN276" s="1"/>
     </row>
     <row r="277" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN277" s="1"/>
     </row>
-    <row r="278" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN278" s="1"/>
-    </row>
-    <row r="279" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN279" s="1"/>
-    </row>
     <row r="280" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN280" s="1"/>
     </row>
@@ -19823,6 +19820,12 @@
     <row r="290" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN290" s="1"/>
     </row>
+    <row r="291" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN291" s="1"/>
+    </row>
+    <row r="292" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN292" s="1"/>
+    </row>
     <row r="293" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN293" s="1"/>
     </row>
@@ -19895,15 +19898,6 @@
     <row r="316" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN316" s="1"/>
     </row>
-    <row r="317" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN317" s="1"/>
-    </row>
-    <row r="318" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN318" s="1"/>
-    </row>
-    <row r="319" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN319" s="1"/>
-    </row>
     <row r="320" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN320" s="1"/>
     </row>
@@ -19913,53 +19907,23 @@
     <row r="322" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN322" s="1"/>
     </row>
-    <row r="323" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN323" s="1"/>
-    </row>
-    <row r="324" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN324" s="1"/>
-    </row>
-    <row r="325" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN325" s="1"/>
-    </row>
-    <row r="326" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN326" s="1"/>
-    </row>
-    <row r="327" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN327" s="1"/>
-    </row>
-    <row r="328" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN328" s="1"/>
-    </row>
-    <row r="329" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN329" s="1"/>
-    </row>
-    <row r="333" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN333" s="1"/>
-    </row>
-    <row r="334" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN334" s="1"/>
-    </row>
-    <row r="335" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN335" s="1"/>
-    </row>
-    <row r="364" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN364" s="1"/>
-    </row>
-    <row r="387" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN387" s="1"/>
-    </row>
-    <row r="388" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN388" s="1"/>
-    </row>
-    <row r="389" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN389" s="1"/>
-    </row>
-    <row r="390" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN390" s="1"/>
+    <row r="351" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN351" s="1"/>
+    </row>
+    <row r="374" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN374" s="1"/>
+    </row>
+    <row r="375" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN375" s="1"/>
+    </row>
+    <row r="376" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN376" s="1"/>
+    </row>
+    <row r="377" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN377" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AV391">
+  <autoFilter ref="A1:AV378">
     <sortState ref="A2:AV391">
       <sortCondition ref="A1:A391"/>
     </sortState>

</xml_diff>